<commit_message>
Updated solarwindsbioshop Excel sheet
</commit_message>
<xml_diff>
--- a/solarwindbioshop.xlsx
+++ b/solarwindbioshop.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jvhaarst/Google Drive/code/solar_scrape/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE8F8F9-2AEC-9F4C-BF54-EB679F790DDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CAE1863-F945-4E4E-9D2C-C2784FE7CAAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="20180" xr2:uid="{B7DBFAC2-7F2D-E44C-8457-AD95CC61E5E5}"/>
   </bookViews>
@@ -23,18 +23,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="35">
   <si>
     <t>Naam</t>
   </si>
@@ -51,142 +45,94 @@
     <t>power</t>
   </si>
   <si>
-    <t xml:space="preserve">JA Solar  - Poly - half cell  Poly 285 Wp </t>
-  </si>
-  <si>
     <t>solarwindbioshop</t>
   </si>
   <si>
     <t>http://www.solarwindbioshop.com/EnerShop-ZONNEPANELEN.htm</t>
   </si>
   <si>
-    <t xml:space="preserve">Jinko Solar  - Cheetah Mono 305 Wp Full Black </t>
-  </si>
-  <si>
-    <t>Jinko Solar  - Cheetah Mono 315 Wp alu frame</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BOVIET  Poly   285  Wp </t>
-  </si>
-  <si>
-    <t>Canadian Solar   half cel Poly 290 Wp  Poly</t>
-  </si>
-  <si>
-    <t>JA-Solar   + SE  Poly 270 Wp  met SE Optimizer</t>
-  </si>
-  <si>
-    <t>Canadian Solar     (HiKu)   KINGSIZE  405 Wp Poly</t>
-  </si>
-  <si>
-    <t>JA Solar     (Mono-PERC°-halfcell)   KINGSIZE 405 Wp Mono</t>
-  </si>
-  <si>
-    <t>JA-Solar  starters modules  Poly 275 Wp -5BB  (Cypress- 35 mm)</t>
-  </si>
-  <si>
-    <t>Mono 310 Wp zwart frame 305 Wp All Black + SE</t>
-  </si>
-  <si>
-    <t>Canadian Solar         300 Wp Mono Full Black                      </t>
-  </si>
-  <si>
-    <t>JA SOLARMono 300 Wp All Black  + SE</t>
-  </si>
-  <si>
-    <t>JA SOLARMono 300 Wp  All Black </t>
-  </si>
-  <si>
-    <t>JA SOLARMono 310 Wp zwart frame </t>
-  </si>
-  <si>
-    <t>BOVIET300 Wp Mono, zwart frame</t>
-  </si>
-  <si>
-    <t>LONGI SOLAR 5BBMono 305 Wp All Black</t>
-  </si>
-  <si>
-    <t>LONGI SOLAR 5BBMono 315 Wp "halfcell" All Black</t>
-  </si>
-  <si>
-    <t>URE310 Wp Mono Full Black</t>
-  </si>
-  <si>
-    <t>URE330 Wp Mono , alu frame</t>
-  </si>
-  <si>
-    <t>JA SOLAR  Mono PERC°  bifacial (glas-glas)Mono 375 Wp glas-glas (zwart frame)</t>
-  </si>
-  <si>
-    <t>Canadian Solar HiDM  Mono PERC°   All BlackMono Full Black 325 Wp</t>
-  </si>
-  <si>
-    <t>Seraphim Eclipse All BlackMono Full Black 325 Wp</t>
-  </si>
-  <si>
-    <t>Seraphim Eclipse All BlackMono Full Black 330 Wp</t>
-  </si>
-  <si>
-    <t>Seraphim Eclipse All BlackMono zw. frame 335 Wp</t>
-  </si>
-  <si>
-    <t>BOVIET Full BlackMono Full Black 340 Wp</t>
-  </si>
-  <si>
-    <t>BOVIET Full BlackMono zw. frame 345 Wp</t>
-  </si>
-  <si>
-    <t>Q CELLS   DUO 325 Wp Mono, zwart frame</t>
-  </si>
-  <si>
-    <t>Q CELLS   DUO 300 Wp Mono, Full Black</t>
-  </si>
-  <si>
-    <t>LG Neon 2  A5330 Wp  Mono Black Frame</t>
-  </si>
-  <si>
-    <t>LG Neon 2  A6350 Wp  Mono Black Frame</t>
-  </si>
-  <si>
-    <t>LG Neon 2  A7400 Wp  Mono bifacial  (kingsize)</t>
-  </si>
-  <si>
-    <t>LG Neon2Black  Chello330 Wp  Mono Full Black</t>
-  </si>
-  <si>
-    <t>LG Neon2Black  Chello335 Wp  Mono Full Black</t>
-  </si>
-  <si>
-    <t>AUO (vh BenQ)    SunBravoMono 330 Wp zwart frame</t>
-  </si>
-  <si>
-    <t>AUO (vh BenQ)    SunBravoMono 320 Wp Full Black</t>
-  </si>
-  <si>
-    <t>PanasonicMono 325 Wp zwart </t>
-  </si>
-  <si>
-    <t>PanasonicMono 330 Wp zwart </t>
-  </si>
-  <si>
-    <t>Avancis "design panel"</t>
-  </si>
-  <si>
-    <t>LONGI SOLAR 5BB 350 Wp,Mono, zw. fr.</t>
-  </si>
-  <si>
-    <t>LONGI SOLAR 5BB 320 Wp, Mono</t>
-  </si>
-  <si>
-    <t>QCELLS   (Peak-Duo)  335 Wp Mono Full Black</t>
-  </si>
-  <si>
-    <t>DENIM Full Black Mono Full Black 305 Wp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DENIM Mono zw. frame glas/glas 315 Wp </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DENIM Full Black KINGSIZE , 72 cells Mono Full Black 380 Wp </t>
+    <t xml:space="preserve">JINKO Tiger serie 350 Wp  Mono, halfcel, All Black Mono 350 Wp Mono, hc, AB </t>
+  </si>
+  <si>
+    <t>JA-Solar   modules met geintegreerde optimizer Mono 325 Wp  met SE Optimizer</t>
+  </si>
+  <si>
+    <t>JA Solar  (Mono-PERC°-halfcell)  415 Wp Mono   Alu frame</t>
+  </si>
+  <si>
+    <t>JA Solar  315 Wp All Black + SE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canadian Solar  half cel   KuBlack  310 Wp Mono Full Black </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JA SOLAR Mono 325 Wp  All Black </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JA SOLAR Mono 365 Wp  All Black </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JA SOLAR Mono 345 Wp  All Black </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JA SOLAR Mono 380 Wp  All Black </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JA SOLAR Mono 385 Wp  All Black </t>
+  </si>
+  <si>
+    <t>LONGI SOLAR  5BB Mono 360 Wp, hc,  All Black</t>
+  </si>
+  <si>
+    <t>LONGI SOLAR  5BB Mono 365 Wp, hc,  All Black</t>
+  </si>
+  <si>
+    <t xml:space="preserve">URE 350 Wp Mono Full Black </t>
+  </si>
+  <si>
+    <t xml:space="preserve">URE 320 Wp Mono Full Black </t>
+  </si>
+  <si>
+    <t>QCELLS   (Peak-Duo)  340 Wp Mono Full Black</t>
+  </si>
+  <si>
+    <t>JA SOLAR     halfcel Mono, hc, SF  460 Wp</t>
+  </si>
+  <si>
+    <t>JA SOLAR     halfcel Mono, hc, SF  495 Wp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JA SOLAR  Mono PERC°  bifacial (glas-glas)  Mono 410 Wp glas-glas (alu frame) </t>
+  </si>
+  <si>
+    <t>Canadian Solar HiKU  Mono PERC°  alu frame Mono 365 Wp HiKU°</t>
+  </si>
+  <si>
+    <t>AEG  glas/glas  Full Black Mono 325 Wp</t>
+  </si>
+  <si>
+    <t>LG Neon 2 330 Wp  Mono Black Frame</t>
+  </si>
+  <si>
+    <t>LG Neon 2 350 Wp  Mono Black Frame</t>
+  </si>
+  <si>
+    <t>LG Neon 2 400 Wp  Mono Black Frame</t>
+  </si>
+  <si>
+    <t>LG Neon2Black  Chello 330 Wp  Mono Full Black</t>
+  </si>
+  <si>
+    <t>LG Neon2Black  Chello 335 Wp  Mono Full Black</t>
+  </si>
+  <si>
+    <t>Panasonic Mono 325 Wp Mono Full Black</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panasonic Mono 330 Wp Mono, zwart frame </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avancis "design panel"  CIS module 145 Wp  Gitzwart </t>
   </si>
 </sst>
 </file>
@@ -544,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{051A0941-3A38-4F4B-95F6-14978B09175E}">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -578,19 +524,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2">
-        <v>97</v>
+        <v>139</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2">
-        <v>285</v>
+        <v>350</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -598,16 +544,16 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>132</v>
+        <v>158</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3">
-        <v>305</v>
+        <v>325</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -615,16 +561,16 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E4">
-        <v>315</v>
+        <v>415</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -632,16 +578,16 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>98</v>
+        <v>156</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5">
-        <v>285</v>
+        <v>315</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -649,84 +595,84 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E6">
-        <v>290</v>
+        <v>310</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B7">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E7">
-        <v>275</v>
+        <v>325</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8">
-        <v>270</v>
+        <v>365</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9">
-        <v>154</v>
+        <v>122</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E9">
-        <v>405</v>
+        <v>345</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10">
-        <v>154</v>
+        <v>134</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E10">
-        <v>405</v>
+        <v>380</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -734,16 +680,16 @@
         <v>16</v>
       </c>
       <c r="B11">
-        <v>175</v>
+        <v>137</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E11">
-        <v>305</v>
+        <v>385</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -751,16 +697,16 @@
         <v>17</v>
       </c>
       <c r="B12">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E12">
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -768,16 +714,16 @@
         <v>18</v>
       </c>
       <c r="B13">
-        <v>172</v>
+        <v>130</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E13">
-        <v>300</v>
+        <v>365</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -785,16 +731,16 @@
         <v>19</v>
       </c>
       <c r="B14">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E14">
-        <v>300</v>
+        <v>350</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -802,16 +748,16 @@
         <v>20</v>
       </c>
       <c r="B15">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E15">
-        <v>310</v>
+        <v>320</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -819,16 +765,16 @@
         <v>21</v>
       </c>
       <c r="B16">
-        <v>126</v>
+        <v>158</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E16">
-        <v>300</v>
+        <v>340</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -836,16 +782,16 @@
         <v>22</v>
       </c>
       <c r="B17">
-        <v>131</v>
+        <v>167</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E17">
-        <v>305</v>
+        <v>460</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -853,166 +799,166 @@
         <v>23</v>
       </c>
       <c r="B18">
-        <v>142</v>
+        <v>185</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E18">
-        <v>315</v>
+        <v>495</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="B19">
-        <v>125</v>
+        <v>149</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E19">
-        <v>320</v>
+        <v>410</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="B20">
-        <v>151</v>
+        <v>122</v>
       </c>
       <c r="C20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E20">
-        <v>350</v>
+        <v>365</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="B21">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E21">
-        <v>335</v>
+        <v>325</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B22">
-        <v>128</v>
+        <v>209</v>
       </c>
       <c r="C22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E22">
-        <v>310</v>
+        <v>330</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B23">
-        <v>126</v>
+        <v>249</v>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E23">
-        <v>330</v>
+        <v>350</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B24">
-        <v>166</v>
+        <v>317</v>
       </c>
       <c r="C24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E24">
-        <v>375</v>
+        <v>400</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B25">
-        <v>172</v>
+        <v>236</v>
       </c>
       <c r="C25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E25">
-        <v>325</v>
+        <v>330</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B26">
-        <v>140</v>
+        <v>245</v>
       </c>
       <c r="C26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E26">
-        <v>325</v>
+        <v>335</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B27">
-        <v>152</v>
+        <v>238</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E27">
         <v>330</v>
@@ -1020,357 +966,69 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B28">
-        <v>141</v>
+        <v>247</v>
       </c>
       <c r="C28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E28">
-        <v>335</v>
+        <v>325</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B29">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="C29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E29">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30">
-        <v>157</v>
-      </c>
-      <c r="C30" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>33</v>
-      </c>
-      <c r="B31">
-        <v>168</v>
-      </c>
-      <c r="C31" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32">
-        <v>145</v>
-      </c>
-      <c r="C32" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" t="s">
-        <v>7</v>
-      </c>
-      <c r="E32">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>48</v>
-      </c>
-      <c r="B33">
-        <v>151</v>
-      </c>
-      <c r="C33" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" t="s">
-        <v>7</v>
-      </c>
-      <c r="E33">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>49</v>
-      </c>
-      <c r="B34">
-        <v>163</v>
-      </c>
-      <c r="C34" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" t="s">
-        <v>7</v>
-      </c>
-      <c r="E34">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>50</v>
-      </c>
-      <c r="B35">
-        <v>204</v>
-      </c>
-      <c r="C35" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E35">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36">
-        <v>209</v>
-      </c>
-      <c r="C36" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" t="s">
-        <v>7</v>
-      </c>
-      <c r="E36">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>36</v>
-      </c>
-      <c r="B37">
-        <v>249</v>
-      </c>
-      <c r="C37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" t="s">
-        <v>7</v>
-      </c>
-      <c r="E37">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38">
-        <v>317</v>
-      </c>
-      <c r="C38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" t="s">
-        <v>7</v>
-      </c>
-      <c r="E38">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>38</v>
-      </c>
-      <c r="B39">
-        <v>236</v>
-      </c>
-      <c r="C39" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>39</v>
-      </c>
-      <c r="B40">
-        <v>245</v>
-      </c>
-      <c r="C40" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" t="s">
-        <v>7</v>
-      </c>
-      <c r="E40">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>40</v>
-      </c>
-      <c r="B41">
-        <v>174</v>
-      </c>
-      <c r="C41" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>41</v>
-      </c>
-      <c r="B42">
-        <v>171</v>
-      </c>
-      <c r="C42" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42" t="s">
-        <v>7</v>
-      </c>
-      <c r="E42">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>42</v>
-      </c>
-      <c r="B43">
-        <v>220</v>
-      </c>
-      <c r="C43" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" t="s">
-        <v>7</v>
-      </c>
-      <c r="E43">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>43</v>
-      </c>
-      <c r="B44">
-        <v>255</v>
-      </c>
-      <c r="C44" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" t="s">
-        <v>7</v>
-      </c>
-      <c r="E44">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>44</v>
-      </c>
-      <c r="B45">
-        <v>135</v>
-      </c>
-      <c r="C45" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" t="s">
-        <v>7</v>
-      </c>
-      <c r="E45">
         <v>145</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{FA5E8C0A-5E78-FA47-AF4F-905F6B476964}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{0C641DB0-4BFC-9149-8A9C-CC0EAB6F981F}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{480D65FE-E331-7548-94A4-5EB7D49BBE30}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{F0BAE08B-A177-C245-B9FE-261E16F07679}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{FF9BBDBA-6F8F-1841-BAB0-4F46F2951A36}"/>
-    <hyperlink ref="D7" r:id="rId6" xr:uid="{DE0F02BA-25B5-884A-B573-F512D49A3F03}"/>
-    <hyperlink ref="D8" r:id="rId7" xr:uid="{26310590-4C38-C644-A201-326D59356B4B}"/>
-    <hyperlink ref="D9" r:id="rId8" xr:uid="{A365C83D-078E-3547-A2E6-987CF2CD7570}"/>
-    <hyperlink ref="D10" r:id="rId9" xr:uid="{C8119003-ECE9-ED44-B537-34F91BCE03E0}"/>
-    <hyperlink ref="D11" r:id="rId10" xr:uid="{9B683E92-A160-EF43-8B1C-AD4528F005C2}"/>
-    <hyperlink ref="D12" r:id="rId11" xr:uid="{A9D82015-FECA-AC42-A427-202A63B0ABD4}"/>
-    <hyperlink ref="D13" r:id="rId12" xr:uid="{B6E7E07B-CF71-F844-80D3-C19893894C36}"/>
-    <hyperlink ref="D14" r:id="rId13" xr:uid="{F2D8DA92-6D94-B34D-82A0-9E9C52CAEC39}"/>
-    <hyperlink ref="D15" r:id="rId14" xr:uid="{BD5003A8-A858-FE44-8F95-F579B442140B}"/>
-    <hyperlink ref="D16" r:id="rId15" xr:uid="{5879E437-A1A5-1448-8430-4B9ECC2EC2D7}"/>
-    <hyperlink ref="D17" r:id="rId16" xr:uid="{7C6ECF9E-CAAC-7747-8EAF-322C3418F30D}"/>
-    <hyperlink ref="D18" r:id="rId17" xr:uid="{2F543876-F934-4042-8AAB-0A398485DEC6}"/>
-    <hyperlink ref="D22" r:id="rId18" xr:uid="{ED1AC83F-F45E-AE49-A9CE-4B252145D7AE}"/>
-    <hyperlink ref="D23" r:id="rId19" xr:uid="{C38989E2-A433-D648-8D45-8F209B93261A}"/>
-    <hyperlink ref="D24" r:id="rId20" xr:uid="{ACC8E6AB-3BD3-D64D-AD0D-BBF25247459F}"/>
-    <hyperlink ref="D25" r:id="rId21" xr:uid="{4C85349A-5311-B348-909B-E99B394F9516}"/>
-    <hyperlink ref="D26" r:id="rId22" xr:uid="{20BD5D6D-31DB-D741-8B8E-D9FBDF1327DC}"/>
-    <hyperlink ref="D27" r:id="rId23" xr:uid="{6051ECD3-9025-DF44-AFBA-FCD5EEF3C8A6}"/>
-    <hyperlink ref="D28" r:id="rId24" xr:uid="{FA93487B-29C0-2542-B405-A9B75FBAA66E}"/>
-    <hyperlink ref="D29" r:id="rId25" xr:uid="{0F354D32-C8F9-2E4A-A19C-9F71B64D9FD3}"/>
-    <hyperlink ref="D30" r:id="rId26" xr:uid="{7A1BB5C6-1921-0B46-9E91-AFACC1C16B0C}"/>
-    <hyperlink ref="D31" r:id="rId27" xr:uid="{3041040F-8FB4-6D42-B86A-41B53D953730}"/>
-    <hyperlink ref="D32" r:id="rId28" xr:uid="{33DEAAA5-AAEA-8F4A-BF6B-7697FFBC6328}"/>
-    <hyperlink ref="D36" r:id="rId29" xr:uid="{31A4AE0C-04E2-4446-8315-8E08123D63E4}"/>
-    <hyperlink ref="D37" r:id="rId30" xr:uid="{82D99AF8-8313-184D-B443-D00A2297C905}"/>
-    <hyperlink ref="D38" r:id="rId31" xr:uid="{E3ECCE0B-CC26-C940-BCC9-1B14F61029AB}"/>
-    <hyperlink ref="D39" r:id="rId32" xr:uid="{FFD25BAB-4500-C642-87E5-DA561CEB57ED}"/>
-    <hyperlink ref="D40" r:id="rId33" xr:uid="{BBA10A31-9DCA-5443-A8F2-9424F555212F}"/>
-    <hyperlink ref="D41" r:id="rId34" xr:uid="{4F97E380-67BB-A849-87C3-042842C19C19}"/>
-    <hyperlink ref="D42" r:id="rId35" xr:uid="{B6BACF8C-56DE-6542-A7C3-9129E0B93CEB}"/>
-    <hyperlink ref="D43" r:id="rId36" xr:uid="{CB9E71DE-58B4-3548-A54A-424189F33446}"/>
-    <hyperlink ref="D44" r:id="rId37" xr:uid="{BB5286C1-06B7-A94F-9C09-8798DF0E88B2}"/>
-    <hyperlink ref="D45" r:id="rId38" xr:uid="{2ACF918B-3F2C-5347-92FA-CF7903BB08BC}"/>
-    <hyperlink ref="D19" r:id="rId39" xr:uid="{9EF87EB3-B6B5-FC4C-96AF-97198499BCA7}"/>
-    <hyperlink ref="D20" r:id="rId40" xr:uid="{B9714859-E3C5-1B47-ABF2-944A04E40A9E}"/>
-    <hyperlink ref="D21" r:id="rId41" xr:uid="{00D392D8-C12D-B244-AE8A-7DE4C4E2B381}"/>
-    <hyperlink ref="D33" r:id="rId42" xr:uid="{E5646BC7-F5ED-1F48-93B2-400BD6BE9A08}"/>
-    <hyperlink ref="D34" r:id="rId43" xr:uid="{2F6C74F7-8BE1-094F-AD7D-A3FF978B4FD6}"/>
-    <hyperlink ref="D35" r:id="rId44" xr:uid="{0BA3F56C-A5AF-E443-BDBE-3B5E54A72B1E}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{46503CD7-E428-824D-87F5-011B5BFCB256}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{66F9495B-CEC2-534E-B7A7-9BD67411340A}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{BDC4D3E1-1E6F-7841-8F55-AD1356E3B4BA}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{B84133CA-83CF-F447-9147-50B17620F521}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{0F58299E-A9EC-C04D-BBC0-A2250301F806}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{C66C1115-FA98-9C43-AD86-2103222DF53A}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{0E7815C9-A78C-9F47-A7AA-FC7F8BA43BCF}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{DBE2E4A4-AFF4-0043-B70B-A8CC31DCD9B6}"/>
+    <hyperlink ref="D10" r:id="rId9" xr:uid="{1097672E-EE6E-EE4E-B219-A90A48A2E9E2}"/>
+    <hyperlink ref="D11" r:id="rId10" xr:uid="{021DCCDE-A60D-1D44-B98C-0F8C179F0A64}"/>
+    <hyperlink ref="D12" r:id="rId11" xr:uid="{4E413A36-E1CD-7D49-9F9A-F5C72C8E711A}"/>
+    <hyperlink ref="D13" r:id="rId12" xr:uid="{38E44255-1CAF-B448-90F9-B9A3CAF94D71}"/>
+    <hyperlink ref="D14" r:id="rId13" xr:uid="{E1A0ABDE-820F-1442-8C34-99E53749EF7A}"/>
+    <hyperlink ref="D15" r:id="rId14" xr:uid="{8DDD6FB9-FF48-AF43-B1F4-38B175C9BB9A}"/>
+    <hyperlink ref="D16" r:id="rId15" xr:uid="{6F9564EC-0E54-5644-BEDE-75CD3716B27C}"/>
+    <hyperlink ref="D17" r:id="rId16" xr:uid="{C439D0A9-F0AF-0B44-A2DD-D64A4A61E7DD}"/>
+    <hyperlink ref="D18" r:id="rId17" xr:uid="{0E3B6871-8F8C-1A46-8640-A6E224AD3B64}"/>
+    <hyperlink ref="D19" r:id="rId18" xr:uid="{41A9E3AF-D55C-A74D-951E-993464A11C6E}"/>
+    <hyperlink ref="D20" r:id="rId19" xr:uid="{145AE1BE-FB16-EA4B-AE60-3F236C98ED42}"/>
+    <hyperlink ref="D21" r:id="rId20" xr:uid="{A94192E2-A394-6848-BC12-4536192FCB92}"/>
+    <hyperlink ref="D22" r:id="rId21" xr:uid="{E1091097-5ED9-8544-AB27-12138C017BA9}"/>
+    <hyperlink ref="D23" r:id="rId22" xr:uid="{074D86E3-C4F1-B04A-9794-36B619B5A2CE}"/>
+    <hyperlink ref="D24" r:id="rId23" xr:uid="{629D6AA0-B160-A949-9131-E9FC28994CA2}"/>
+    <hyperlink ref="D25" r:id="rId24" xr:uid="{8BE4A048-EABF-4A4B-9446-0BA760995A22}"/>
+    <hyperlink ref="D26" r:id="rId25" xr:uid="{AE7EC865-4C48-E540-A025-A4C54D23C865}"/>
+    <hyperlink ref="D27" r:id="rId26" xr:uid="{FB343C3B-2C0F-6C41-A31F-1FBDBF409178}"/>
+    <hyperlink ref="D28" r:id="rId27" xr:uid="{0231603B-D480-834B-8AF0-55BAC6749373}"/>
+    <hyperlink ref="D29" r:id="rId28" xr:uid="{F65766D1-ED0B-DA4D-A4B9-CCA856B76E2A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>